<commit_message>
Few bugs fixed -all numbers(non admins) publicOnly: true and numbers administration filter kept when approved /disapprove number
</commit_message>
<xml_diff>
--- a/Web/UserEx.Web/wwwroot/Files/CDRs-05_11_09_2022-58_Test - Copy (2).xlsx
+++ b/Web/UserEx.Web/wwwroot/Files/CDRs-05_11_09_2022-58_Test - Copy (2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://naxex-my.sharepoint.com/personal/emil_hristov_tiebreak_solutions/Documents/Stuff/coding/ASP.NET/UseEx_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{867C3A93-C833-4AAB-8187-8B2A052F3F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A76211B5-AD62-4A4F-AB3B-AA4E453761FA}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{867C3A93-C833-4AAB-8187-8B2A052F3F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{233E95CF-DD54-420D-BD01-B4F5724CCAF9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDRs-05_11_09_2022-58" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>DIDlogic</t>
+  </si>
+  <si>
+    <t>Bezeq</t>
   </si>
 </sst>
 </file>
@@ -932,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:G160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="L161" sqref="L161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4603,6 +4606,29 @@
       </c>
       <c r="G159" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>44901.81517361111</v>
+      </c>
+      <c r="B160" s="2">
+        <v>551148582910</v>
+      </c>
+      <c r="C160" s="2">
+        <v>448455642100</v>
+      </c>
+      <c r="D160">
+        <v>58424</v>
+      </c>
+      <c r="E160">
+        <v>5</v>
+      </c>
+      <c r="F160">
+        <v>157</v>
+      </c>
+      <c r="G160" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>